<commit_message>
Removing 2.3 from checklist
Per https://github.com/OWASP/ASVS/issues/201
</commit_message>
<xml_diff>
--- a/3.0.1/OWASP Application Security Verification Standard Checklist 3.0.1.xlsx
+++ b/3.0.1/OWASP Application Security Verification Standard Checklist 3.0.1.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27224"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10709"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmanico/workspace/ASVS/3.0.1/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5B60236-6FCF-6944-8ECF-FE5B5ABDB115}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25220" windowHeight="14520" activeTab="2"/>
+    <workbookView xWindow="2260" yWindow="460" windowWidth="25700" windowHeight="16820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ASVS 3.0.1 Detail Requirements" sheetId="1" r:id="rId1"/>
     <sheet name="What ever happened to ..." sheetId="2" r:id="rId2"/>
     <sheet name="Document and License Info" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1060" uniqueCount="533">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1055" uniqueCount="533">
   <si>
     <t>ID</t>
   </si>
@@ -1639,7 +1640,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -2457,11 +2458,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R987"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:R986"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2649,7 +2650,7 @@
       </c>
       <c r="G9" s="14"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:18" ht="26" x14ac:dyDescent="0.15">
       <c r="A10" s="9" t="s">
         <v>24</v>
       </c>
@@ -2904,7 +2905,7 @@
       </c>
       <c r="G22" s="26"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A23" s="21" t="s">
         <v>44</v>
       </c>
@@ -3201,16 +3202,14 @@
       </c>
       <c r="G37" s="26"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A38" s="21" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B38" s="22" t="s">
-        <v>70</v>
-      </c>
-      <c r="C38" s="23" t="s">
-        <v>11</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="C38" s="27"/>
       <c r="D38" s="24" t="s">
         <v>11</v>
       </c>
@@ -3222,14 +3221,16 @@
       </c>
       <c r="G38" s="26"/>
     </row>
-    <row r="39" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A39" s="21" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B39" s="22" t="s">
-        <v>72</v>
-      </c>
-      <c r="C39" s="27"/>
+        <v>74</v>
+      </c>
+      <c r="C39" s="23" t="s">
+        <v>11</v>
+      </c>
       <c r="D39" s="24" t="s">
         <v>11</v>
       </c>
@@ -3242,11 +3243,11 @@
       <c r="G39" s="26"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A40" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="B40" s="22" t="s">
-        <v>74</v>
+      <c r="A40" s="46" t="s">
+        <v>508</v>
+      </c>
+      <c r="B40" s="65" t="s">
+        <v>509</v>
       </c>
       <c r="C40" s="23" t="s">
         <v>11</v>
@@ -3257,51 +3258,51 @@
       <c r="E40" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="F40" s="69">
-        <v>3</v>
+      <c r="F40" s="70" t="s">
+        <v>499</v>
       </c>
       <c r="G40" s="26"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A41" s="46" t="s">
-        <v>508</v>
-      </c>
-      <c r="B41" s="65" t="s">
-        <v>509</v>
-      </c>
-      <c r="C41" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="D41" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="E41" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="F41" s="70" t="s">
-        <v>499</v>
-      </c>
-      <c r="G41" s="26"/>
+      <c r="A41" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="B41" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="C41" s="19"/>
+      <c r="D41" s="19"/>
+      <c r="E41" s="19"/>
+      <c r="F41" s="75"/>
+      <c r="G41" s="20"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A42" s="17" t="s">
-        <v>75</v>
-      </c>
-      <c r="B42" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="C42" s="19"/>
-      <c r="D42" s="19"/>
-      <c r="E42" s="19"/>
-      <c r="F42" s="75"/>
-      <c r="G42" s="20"/>
+      <c r="A42" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="B42" s="22" t="s">
+        <v>78</v>
+      </c>
+      <c r="C42" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D42" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E42" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="F42" s="69">
+        <v>1</v>
+      </c>
+      <c r="G42" s="26"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A43" s="21" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B43" s="22" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C43" s="23" t="s">
         <v>11</v>
@@ -3319,10 +3320,10 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A44" s="21" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B44" s="22" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C44" s="23" t="s">
         <v>11</v>
@@ -3340,14 +3341,12 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A45" s="21" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B45" s="22" t="s">
-        <v>82</v>
-      </c>
-      <c r="C45" s="23" t="s">
-        <v>11</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="C45" s="27"/>
       <c r="D45" s="24" t="s">
         <v>11</v>
       </c>
@@ -3361,12 +3360,14 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A46" s="21" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B46" s="22" t="s">
-        <v>84</v>
-      </c>
-      <c r="C46" s="27"/>
+        <v>86</v>
+      </c>
+      <c r="C46" s="23" t="s">
+        <v>11</v>
+      </c>
       <c r="D46" s="24" t="s">
         <v>11</v>
       </c>
@@ -3378,12 +3379,12 @@
       </c>
       <c r="G46" s="26"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A47" s="21" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B47" s="22" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C47" s="23" t="s">
         <v>11</v>
@@ -3399,12 +3400,12 @@
       </c>
       <c r="G47" s="26"/>
     </row>
-    <row r="48" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A48" s="21" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B48" s="22" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C48" s="23" t="s">
         <v>11</v>
@@ -3422,14 +3423,12 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A49" s="21" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B49" s="22" t="s">
-        <v>90</v>
-      </c>
-      <c r="C49" s="23" t="s">
-        <v>11</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="C49" s="27"/>
       <c r="D49" s="24" t="s">
         <v>11</v>
       </c>
@@ -3443,12 +3442,14 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A50" s="21" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B50" s="22" t="s">
-        <v>92</v>
-      </c>
-      <c r="C50" s="27"/>
+        <v>94</v>
+      </c>
+      <c r="C50" s="23" t="s">
+        <v>11</v>
+      </c>
       <c r="D50" s="24" t="s">
         <v>11</v>
       </c>
@@ -3460,12 +3461,12 @@
       </c>
       <c r="G50" s="26"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A51" s="21" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B51" s="22" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C51" s="23" t="s">
         <v>11</v>
@@ -3477,16 +3478,16 @@
         <v>11</v>
       </c>
       <c r="F51" s="69">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G51" s="26"/>
     </row>
-    <row r="52" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A52" s="21" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B52" s="22" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C52" s="23" t="s">
         <v>11</v>
@@ -3504,10 +3505,10 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A53" s="21" t="s">
-        <v>97</v>
-      </c>
-      <c r="B53" s="22" t="s">
-        <v>98</v>
+        <v>99</v>
+      </c>
+      <c r="B53" s="65" t="s">
+        <v>100</v>
       </c>
       <c r="C53" s="23" t="s">
         <v>11</v>
@@ -3525,10 +3526,10 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A54" s="21" t="s">
-        <v>99</v>
-      </c>
-      <c r="B54" s="65" t="s">
-        <v>100</v>
+        <v>101</v>
+      </c>
+      <c r="B54" s="22" t="s">
+        <v>102</v>
       </c>
       <c r="C54" s="23" t="s">
         <v>11</v>
@@ -3545,45 +3546,45 @@
       <c r="G54" s="26"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A55" s="21" t="s">
-        <v>101</v>
-      </c>
-      <c r="B55" s="22" t="s">
-        <v>102</v>
-      </c>
-      <c r="C55" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="D55" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="E55" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="F55" s="69">
-        <v>3</v>
-      </c>
-      <c r="G55" s="26"/>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A56" s="17" t="s">
+      <c r="A55" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="B56" s="18" t="s">
+      <c r="B55" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="C56" s="19"/>
-      <c r="D56" s="19"/>
-      <c r="E56" s="19"/>
-      <c r="F56" s="75"/>
-      <c r="G56" s="20"/>
+      <c r="C55" s="19"/>
+      <c r="D55" s="19"/>
+      <c r="E55" s="19"/>
+      <c r="F55" s="75"/>
+      <c r="G55" s="20"/>
+    </row>
+    <row r="56" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+      <c r="A56" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="B56" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="C56" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D56" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E56" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="F56" s="69">
+        <v>1</v>
+      </c>
+      <c r="G56" s="26"/>
     </row>
     <row r="57" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A57" s="21" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B57" s="22" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C57" s="23" t="s">
         <v>11</v>
@@ -3601,10 +3602,10 @@
     </row>
     <row r="58" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A58" s="21" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B58" s="22" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C58" s="23" t="s">
         <v>11</v>
@@ -3620,12 +3621,12 @@
       </c>
       <c r="G58" s="26"/>
     </row>
-    <row r="59" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A59" s="21" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B59" s="22" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C59" s="23" t="s">
         <v>11</v>
@@ -3643,10 +3644,10 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A60" s="21" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B60" s="22" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C60" s="23" t="s">
         <v>11</v>
@@ -3664,14 +3665,12 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A61" s="21" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B61" s="22" t="s">
-        <v>114</v>
-      </c>
-      <c r="C61" s="23" t="s">
-        <v>11</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="C61" s="27"/>
       <c r="D61" s="24" t="s">
         <v>11</v>
       </c>
@@ -3683,17 +3682,15 @@
       </c>
       <c r="G61" s="26"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A62" s="21" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B62" s="22" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C62" s="27"/>
-      <c r="D62" s="24" t="s">
-        <v>11</v>
-      </c>
+      <c r="D62" s="27"/>
       <c r="E62" s="25" t="s">
         <v>11</v>
       </c>
@@ -3704,29 +3701,33 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A63" s="21" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B63" s="22" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C63" s="27"/>
-      <c r="D63" s="27"/>
+      <c r="D63" s="24" t="s">
+        <v>11</v>
+      </c>
       <c r="E63" s="25" t="s">
         <v>11</v>
       </c>
       <c r="F63" s="69">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G63" s="26"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A64" s="21" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B64" s="22" t="s">
-        <v>120</v>
-      </c>
-      <c r="C64" s="27"/>
+        <v>122</v>
+      </c>
+      <c r="C64" s="23" t="s">
+        <v>11</v>
+      </c>
       <c r="D64" s="24" t="s">
         <v>11</v>
       </c>
@@ -3738,16 +3739,14 @@
       </c>
       <c r="G64" s="26"/>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A65" s="21" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B65" s="22" t="s">
-        <v>122</v>
-      </c>
-      <c r="C65" s="23" t="s">
-        <v>11</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="C65" s="27"/>
       <c r="D65" s="24" t="s">
         <v>11</v>
       </c>
@@ -3761,10 +3760,10 @@
     </row>
     <row r="66" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A66" s="21" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B66" s="22" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="C66" s="27"/>
       <c r="D66" s="24" t="s">
@@ -3774,18 +3773,20 @@
         <v>11</v>
       </c>
       <c r="F66" s="69">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G66" s="26"/>
     </row>
     <row r="67" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A67" s="21" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B67" s="22" t="s">
-        <v>126</v>
-      </c>
-      <c r="C67" s="27"/>
+        <v>128</v>
+      </c>
+      <c r="C67" s="23" t="s">
+        <v>11</v>
+      </c>
       <c r="D67" s="24" t="s">
         <v>11</v>
       </c>
@@ -3798,45 +3799,45 @@
       <c r="G67" s="26"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A68" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="B68" s="22" t="s">
-        <v>128</v>
-      </c>
-      <c r="C68" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="D68" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="E68" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="F68" s="69">
-        <v>3</v>
-      </c>
-      <c r="G68" s="26"/>
+      <c r="A68" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="B68" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="C68" s="19"/>
+      <c r="D68" s="19"/>
+      <c r="E68" s="19"/>
+      <c r="F68" s="75"/>
+      <c r="G68" s="20"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A69" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="B69" s="18" t="s">
-        <v>130</v>
-      </c>
-      <c r="C69" s="19"/>
-      <c r="D69" s="19"/>
-      <c r="E69" s="19"/>
-      <c r="F69" s="75"/>
-      <c r="G69" s="20"/>
+      <c r="A69" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="B69" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="C69" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D69" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E69" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="F69" s="69">
+        <v>1</v>
+      </c>
+      <c r="G69" s="26"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A70" s="21" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B70" s="22" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C70" s="23" t="s">
         <v>11</v>
@@ -3854,10 +3855,10 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A71" s="21" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B71" s="22" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C71" s="23" t="s">
         <v>11</v>
@@ -3875,17 +3876,13 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A72" s="21" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B72" s="22" t="s">
-        <v>136</v>
-      </c>
-      <c r="C72" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="D72" s="24" t="s">
-        <v>11</v>
-      </c>
+        <v>138</v>
+      </c>
+      <c r="C72" s="27"/>
+      <c r="D72" s="27"/>
       <c r="E72" s="25" t="s">
         <v>11</v>
       </c>
@@ -3894,29 +3891,33 @@
       </c>
       <c r="G72" s="26"/>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A73" s="21" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B73" s="22" t="s">
-        <v>138</v>
-      </c>
-      <c r="C73" s="27"/>
-      <c r="D73" s="27"/>
+        <v>140</v>
+      </c>
+      <c r="C73" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D73" s="24" t="s">
+        <v>11</v>
+      </c>
       <c r="E73" s="25" t="s">
         <v>11</v>
       </c>
       <c r="F73" s="69">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G73" s="26"/>
     </row>
-    <row r="74" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A74" s="21" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B74" s="22" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C74" s="23" t="s">
         <v>11</v>
@@ -3934,10 +3935,10 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A75" s="21" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B75" s="22" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C75" s="23" t="s">
         <v>11</v>
@@ -3955,10 +3956,10 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A76" s="21" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B76" s="22" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C76" s="23" t="s">
         <v>11</v>
@@ -3970,37 +3971,37 @@
         <v>11</v>
       </c>
       <c r="F76" s="69">
+        <v>3</v>
+      </c>
+      <c r="G76" s="26"/>
+    </row>
+    <row r="77" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+      <c r="A77" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="B77" s="22" t="s">
+        <v>148</v>
+      </c>
+      <c r="C77" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D77" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E77" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="F77" s="69">
         <v>2</v>
       </c>
-      <c r="G76" s="26"/>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A77" s="21" t="s">
-        <v>145</v>
-      </c>
-      <c r="B77" s="22" t="s">
-        <v>146</v>
-      </c>
-      <c r="C77" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="D77" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="E77" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="F77" s="69">
-        <v>3</v>
-      </c>
       <c r="G77" s="26"/>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A78" s="21" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B78" s="22" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C78" s="23" t="s">
         <v>11</v>
@@ -4018,14 +4019,12 @@
     </row>
     <row r="79" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A79" s="21" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B79" s="22" t="s">
-        <v>150</v>
-      </c>
-      <c r="C79" s="23" t="s">
-        <v>11</v>
-      </c>
+        <v>152</v>
+      </c>
+      <c r="C79" s="27"/>
       <c r="D79" s="24" t="s">
         <v>11</v>
       </c>
@@ -4039,10 +4038,10 @@
     </row>
     <row r="80" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A80" s="21" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B80" s="22" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="C80" s="27"/>
       <c r="D80" s="24" t="s">
@@ -4056,12 +4055,12 @@
       </c>
       <c r="G80" s="26"/>
     </row>
-    <row r="81" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A81" s="21" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B81" s="22" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C81" s="27"/>
       <c r="D81" s="24" t="s">
@@ -4071,16 +4070,16 @@
         <v>11</v>
       </c>
       <c r="F81" s="69">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G81" s="26"/>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:7" ht="39" x14ac:dyDescent="0.15">
       <c r="A82" s="21" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B82" s="22" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="C82" s="27"/>
       <c r="D82" s="24" t="s">
@@ -4094,12 +4093,12 @@
       </c>
       <c r="G82" s="26"/>
     </row>
-    <row r="83" spans="1:7" ht="39" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A83" s="21" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B83" s="22" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C83" s="27"/>
       <c r="D83" s="24" t="s">
@@ -4115,10 +4114,10 @@
     </row>
     <row r="84" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A84" s="21" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="B84" s="22" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C84" s="27"/>
       <c r="D84" s="24" t="s">
@@ -4134,12 +4133,14 @@
     </row>
     <row r="85" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A85" s="21" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B85" s="22" t="s">
-        <v>162</v>
-      </c>
-      <c r="C85" s="27"/>
+        <v>164</v>
+      </c>
+      <c r="C85" s="23" t="s">
+        <v>11</v>
+      </c>
       <c r="D85" s="24" t="s">
         <v>11</v>
       </c>
@@ -4151,16 +4152,14 @@
       </c>
       <c r="G85" s="26"/>
     </row>
-    <row r="86" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A86" s="21" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B86" s="22" t="s">
-        <v>164</v>
-      </c>
-      <c r="C86" s="23" t="s">
-        <v>11</v>
-      </c>
+        <v>166</v>
+      </c>
+      <c r="C86" s="27"/>
       <c r="D86" s="24" t="s">
         <v>11</v>
       </c>
@@ -4174,10 +4173,10 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A87" s="21" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B87" s="22" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C87" s="27"/>
       <c r="D87" s="24" t="s">
@@ -4193,10 +4192,10 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A88" s="21" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B88" s="22" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C88" s="27"/>
       <c r="D88" s="24" t="s">
@@ -4212,10 +4211,10 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A89" s="21" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B89" s="22" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C89" s="27"/>
       <c r="D89" s="24" t="s">
@@ -4229,61 +4228,61 @@
       </c>
       <c r="G89" s="26"/>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A90" s="21" t="s">
-        <v>171</v>
-      </c>
-      <c r="B90" s="22" t="s">
-        <v>172</v>
-      </c>
-      <c r="C90" s="27"/>
-      <c r="D90" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="E90" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="F90" s="69">
-        <v>3</v>
-      </c>
-      <c r="G90" s="26"/>
-    </row>
-    <row r="91" spans="1:7" ht="26" x14ac:dyDescent="0.15">
-      <c r="A91" s="28" t="s">
+    <row r="90" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+      <c r="A90" s="28" t="s">
         <v>173</v>
       </c>
-      <c r="B91" s="29" t="s">
+      <c r="B90" s="29" t="s">
         <v>174</v>
       </c>
-      <c r="C91" s="30"/>
-      <c r="D91" s="30"/>
-      <c r="E91" s="30"/>
-      <c r="F91" s="76"/>
-      <c r="G91" s="31"/>
+      <c r="C90" s="30"/>
+      <c r="D90" s="30"/>
+      <c r="E90" s="30"/>
+      <c r="F90" s="76"/>
+      <c r="G90" s="31"/>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A91" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="B91" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="C91" s="19"/>
+      <c r="D91" s="19"/>
+      <c r="E91" s="19"/>
+      <c r="F91" s="75"/>
+      <c r="G91" s="20"/>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A92" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="B92" s="18" t="s">
-        <v>176</v>
-      </c>
-      <c r="C92" s="19"/>
-      <c r="D92" s="19"/>
-      <c r="E92" s="19"/>
-      <c r="F92" s="75"/>
-      <c r="G92" s="20"/>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A92" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="B92" s="22" t="s">
+        <v>178</v>
+      </c>
+      <c r="C92" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D92" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E92" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="F92" s="69">
+        <v>1</v>
+      </c>
+      <c r="G92" s="26"/>
+    </row>
+    <row r="93" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A93" s="21" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="B93" s="22" t="s">
-        <v>178</v>
-      </c>
-      <c r="C93" s="23" t="s">
-        <v>11</v>
-      </c>
+        <v>180</v>
+      </c>
+      <c r="C93" s="27"/>
       <c r="D93" s="24" t="s">
         <v>11</v>
       </c>
@@ -4295,14 +4294,16 @@
       </c>
       <c r="G93" s="26"/>
     </row>
-    <row r="94" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A94" s="21" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B94" s="22" t="s">
-        <v>180</v>
-      </c>
-      <c r="C94" s="27"/>
+        <v>182</v>
+      </c>
+      <c r="C94" s="23" t="s">
+        <v>11</v>
+      </c>
       <c r="D94" s="24" t="s">
         <v>11</v>
       </c>
@@ -4316,17 +4317,13 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A95" s="21" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B95" s="22" t="s">
-        <v>182</v>
-      </c>
-      <c r="C95" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="D95" s="24" t="s">
-        <v>11</v>
-      </c>
+        <v>184</v>
+      </c>
+      <c r="C95" s="27"/>
+      <c r="D95" s="27"/>
       <c r="E95" s="25" t="s">
         <v>11</v>
       </c>
@@ -4335,15 +4332,17 @@
       </c>
       <c r="G95" s="26"/>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A96" s="21" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B96" s="22" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C96" s="27"/>
-      <c r="D96" s="27"/>
+      <c r="D96" s="24" t="s">
+        <v>11</v>
+      </c>
       <c r="E96" s="25" t="s">
         <v>11</v>
       </c>
@@ -4354,46 +4353,46 @@
     </row>
     <row r="97" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A97" s="21" t="s">
-        <v>185</v>
-      </c>
-      <c r="B97" s="22" t="s">
-        <v>186</v>
+        <v>187</v>
+      </c>
+      <c r="B97" s="65" t="s">
+        <v>510</v>
       </c>
       <c r="C97" s="27"/>
-      <c r="D97" s="24" t="s">
-        <v>11</v>
-      </c>
+      <c r="D97" s="27"/>
       <c r="E97" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="F97" s="69">
-        <v>1</v>
+      <c r="F97" s="70" t="s">
+        <v>499</v>
       </c>
       <c r="G97" s="26"/>
     </row>
-    <row r="98" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A98" s="21" t="s">
-        <v>187</v>
-      </c>
-      <c r="B98" s="65" t="s">
-        <v>510</v>
+        <v>188</v>
+      </c>
+      <c r="B98" s="32" t="s">
+        <v>189</v>
       </c>
       <c r="C98" s="27"/>
-      <c r="D98" s="27"/>
+      <c r="D98" s="24" t="s">
+        <v>11</v>
+      </c>
       <c r="E98" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="F98" s="70" t="s">
-        <v>499</v>
+      <c r="F98" s="69">
+        <v>3</v>
       </c>
       <c r="G98" s="26"/>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A99" s="21" t="s">
-        <v>188</v>
-      </c>
-      <c r="B99" s="32" t="s">
-        <v>189</v>
+        <v>190</v>
+      </c>
+      <c r="B99" s="65" t="s">
+        <v>511</v>
       </c>
       <c r="C99" s="27"/>
       <c r="D99" s="24" t="s">
@@ -4402,17 +4401,17 @@
       <c r="E99" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="F99" s="69">
-        <v>3</v>
+      <c r="F99" s="70" t="s">
+        <v>499</v>
       </c>
       <c r="G99" s="26"/>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A100" s="21" t="s">
-        <v>190</v>
-      </c>
-      <c r="B100" s="65" t="s">
-        <v>511</v>
+        <v>191</v>
+      </c>
+      <c r="B100" s="22" t="s">
+        <v>192</v>
       </c>
       <c r="C100" s="27"/>
       <c r="D100" s="24" t="s">
@@ -4421,22 +4420,20 @@
       <c r="E100" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="F100" s="70" t="s">
-        <v>499</v>
+      <c r="F100" s="69">
+        <v>3</v>
       </c>
       <c r="G100" s="26"/>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A101" s="21" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="B101" s="22" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="C101" s="27"/>
-      <c r="D101" s="24" t="s">
-        <v>11</v>
-      </c>
+      <c r="D101" s="33"/>
       <c r="E101" s="25" t="s">
         <v>11</v>
       </c>
@@ -4445,46 +4442,48 @@
       </c>
       <c r="G101" s="26"/>
     </row>
-    <row r="102" spans="1:7" ht="26" x14ac:dyDescent="0.15">
-      <c r="A102" s="21" t="s">
-        <v>193</v>
-      </c>
-      <c r="B102" s="22" t="s">
-        <v>194</v>
-      </c>
-      <c r="C102" s="27"/>
-      <c r="D102" s="33"/>
-      <c r="E102" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="F102" s="69">
-        <v>3</v>
-      </c>
-      <c r="G102" s="26"/>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A103" s="17" t="s">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A102" s="17" t="s">
         <v>195</v>
       </c>
-      <c r="B103" s="18" t="s">
+      <c r="B102" s="18" t="s">
         <v>196</v>
       </c>
-      <c r="C103" s="19"/>
-      <c r="D103" s="19"/>
-      <c r="E103" s="19"/>
-      <c r="F103" s="75"/>
-      <c r="G103" s="20"/>
-    </row>
-    <row r="104" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+      <c r="C102" s="19"/>
+      <c r="D102" s="19"/>
+      <c r="E102" s="19"/>
+      <c r="F102" s="75"/>
+      <c r="G102" s="20"/>
+    </row>
+    <row r="103" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+      <c r="A103" s="21" t="s">
+        <v>197</v>
+      </c>
+      <c r="B103" s="22" t="s">
+        <v>198</v>
+      </c>
+      <c r="C103" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D103" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E103" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="F103" s="69">
+        <v>1</v>
+      </c>
+      <c r="G103" s="26"/>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A104" s="21" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B104" s="22" t="s">
-        <v>198</v>
-      </c>
-      <c r="C104" s="23" t="s">
-        <v>11</v>
-      </c>
+        <v>200</v>
+      </c>
+      <c r="C104" s="27"/>
       <c r="D104" s="24" t="s">
         <v>11</v>
       </c>
@@ -4498,10 +4497,10 @@
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A105" s="21" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="B105" s="22" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="C105" s="27"/>
       <c r="D105" s="24" t="s">
@@ -4517,10 +4516,10 @@
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A106" s="21" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B106" s="22" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="C106" s="27"/>
       <c r="D106" s="24" t="s">
@@ -4536,10 +4535,10 @@
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A107" s="21" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="B107" s="22" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="C107" s="27"/>
       <c r="D107" s="24" t="s">
@@ -4555,10 +4554,10 @@
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A108" s="21" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="B108" s="22" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C108" s="27"/>
       <c r="D108" s="24" t="s">
@@ -4572,12 +4571,12 @@
       </c>
       <c r="G108" s="26"/>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="109" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A109" s="21" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B109" s="22" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="C109" s="27"/>
       <c r="D109" s="24" t="s">
@@ -4587,35 +4586,33 @@
         <v>11</v>
       </c>
       <c r="F109" s="69">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G109" s="26"/>
     </row>
-    <row r="110" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A110" s="21" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="B110" s="22" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="C110" s="27"/>
-      <c r="D110" s="24" t="s">
-        <v>11</v>
-      </c>
+      <c r="D110" s="27"/>
       <c r="E110" s="25" t="s">
         <v>11</v>
       </c>
       <c r="F110" s="69">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G110" s="26"/>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A111" s="21" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="B111" s="22" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="C111" s="27"/>
       <c r="D111" s="27"/>
@@ -4629,34 +4626,34 @@
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A112" s="21" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="B112" s="22" t="s">
-        <v>214</v>
-      </c>
-      <c r="C112" s="27"/>
-      <c r="D112" s="27"/>
+        <v>216</v>
+      </c>
+      <c r="C112" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D112" s="24" t="s">
+        <v>11</v>
+      </c>
       <c r="E112" s="25" t="s">
         <v>11</v>
       </c>
       <c r="F112" s="69">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G112" s="26"/>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A113" s="21" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B113" s="22" t="s">
-        <v>216</v>
-      </c>
-      <c r="C113" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="D113" s="24" t="s">
-        <v>11</v>
-      </c>
+        <v>218</v>
+      </c>
+      <c r="C113" s="27"/>
+      <c r="D113" s="27"/>
       <c r="E113" s="25" t="s">
         <v>11</v>
       </c>
@@ -4667,10 +4664,10 @@
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A114" s="21" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="B114" s="22" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="C114" s="27"/>
       <c r="D114" s="27"/>
@@ -4683,69 +4680,69 @@
       <c r="G114" s="26"/>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A115" s="21" t="s">
-        <v>219</v>
-      </c>
-      <c r="B115" s="22" t="s">
-        <v>220</v>
-      </c>
-      <c r="C115" s="27"/>
-      <c r="D115" s="27"/>
+      <c r="A115" s="46">
+        <v>8.1300000000000008</v>
+      </c>
+      <c r="B115" s="65" t="s">
+        <v>512</v>
+      </c>
+      <c r="C115" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D115" s="24" t="s">
+        <v>11</v>
+      </c>
       <c r="E115" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="F115" s="69">
-        <v>3</v>
+      <c r="F115" s="70" t="s">
+        <v>499</v>
       </c>
       <c r="G115" s="26"/>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A116" s="46">
-        <v>8.1300000000000008</v>
-      </c>
-      <c r="B116" s="65" t="s">
-        <v>512</v>
-      </c>
-      <c r="C116" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="D116" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="E116" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="F116" s="70" t="s">
-        <v>499</v>
-      </c>
-      <c r="G116" s="26"/>
+      <c r="A116" s="17" t="s">
+        <v>221</v>
+      </c>
+      <c r="B116" s="18" t="s">
+        <v>222</v>
+      </c>
+      <c r="C116" s="19"/>
+      <c r="D116" s="19"/>
+      <c r="E116" s="19"/>
+      <c r="F116" s="75"/>
+      <c r="G116" s="20"/>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A117" s="17" t="s">
-        <v>221</v>
-      </c>
-      <c r="B117" s="18" t="s">
-        <v>222</v>
-      </c>
-      <c r="C117" s="19"/>
-      <c r="D117" s="19"/>
-      <c r="E117" s="19"/>
-      <c r="F117" s="75"/>
-      <c r="G117" s="20"/>
-    </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A117" s="21" t="s">
+        <v>223</v>
+      </c>
+      <c r="B117" s="22" t="s">
+        <v>224</v>
+      </c>
+      <c r="C117" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D117" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E117" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="F117" s="69">
+        <v>1</v>
+      </c>
+      <c r="G117" s="26"/>
+    </row>
+    <row r="118" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A118" s="21" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="B118" s="22" t="s">
-        <v>224</v>
-      </c>
-      <c r="C118" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="D118" s="24" t="s">
-        <v>11</v>
-      </c>
+        <v>226</v>
+      </c>
+      <c r="C118" s="27"/>
+      <c r="D118" s="27"/>
       <c r="E118" s="25" t="s">
         <v>11</v>
       </c>
@@ -4754,15 +4751,19 @@
       </c>
       <c r="G118" s="26"/>
     </row>
-    <row r="119" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A119" s="21" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="B119" s="22" t="s">
-        <v>226</v>
-      </c>
-      <c r="C119" s="27"/>
-      <c r="D119" s="27"/>
+        <v>228</v>
+      </c>
+      <c r="C119" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D119" s="24" t="s">
+        <v>11</v>
+      </c>
       <c r="E119" s="25" t="s">
         <v>11</v>
       </c>
@@ -4771,12 +4772,12 @@
       </c>
       <c r="G119" s="26"/>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="120" spans="1:7" ht="78" x14ac:dyDescent="0.15">
       <c r="A120" s="21" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="B120" s="22" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="C120" s="23" t="s">
         <v>11</v>
@@ -4792,16 +4793,14 @@
       </c>
       <c r="G120" s="26"/>
     </row>
-    <row r="121" spans="1:7" ht="78" x14ac:dyDescent="0.15">
+    <row r="121" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A121" s="21" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="B121" s="22" t="s">
-        <v>230</v>
-      </c>
-      <c r="C121" s="23" t="s">
-        <v>11</v>
-      </c>
+        <v>232</v>
+      </c>
+      <c r="C121" s="27"/>
       <c r="D121" s="24" t="s">
         <v>11</v>
       </c>
@@ -4813,17 +4812,15 @@
       </c>
       <c r="G121" s="26"/>
     </row>
-    <row r="122" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A122" s="21" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="B122" s="22" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="C122" s="27"/>
-      <c r="D122" s="24" t="s">
-        <v>11</v>
-      </c>
+      <c r="D122" s="27"/>
       <c r="E122" s="25" t="s">
         <v>11</v>
       </c>
@@ -4834,32 +4831,32 @@
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A123" s="21" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="B123" s="22" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="C123" s="27"/>
-      <c r="D123" s="27"/>
+      <c r="D123" s="24" t="s">
+        <v>11</v>
+      </c>
       <c r="E123" s="25" t="s">
         <v>11</v>
       </c>
       <c r="F123" s="69">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G123" s="26"/>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A124" s="21" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="B124" s="22" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="C124" s="27"/>
-      <c r="D124" s="24" t="s">
-        <v>11</v>
-      </c>
+      <c r="D124" s="27"/>
       <c r="E124" s="25" t="s">
         <v>11</v>
       </c>
@@ -4868,50 +4865,52 @@
       </c>
       <c r="G124" s="26"/>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="125" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A125" s="21" t="s">
-        <v>237</v>
-      </c>
-      <c r="B125" s="22" t="s">
-        <v>238</v>
-      </c>
-      <c r="C125" s="27"/>
-      <c r="D125" s="27"/>
+        <v>239</v>
+      </c>
+      <c r="B125" s="65" t="s">
+        <v>513</v>
+      </c>
+      <c r="C125" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D125" s="24" t="s">
+        <v>11</v>
+      </c>
       <c r="E125" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="F125" s="69">
-        <v>2</v>
+      <c r="F125" s="70" t="s">
+        <v>499</v>
       </c>
       <c r="G125" s="26"/>
     </row>
-    <row r="126" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A126" s="21" t="s">
-        <v>239</v>
-      </c>
-      <c r="B126" s="65" t="s">
-        <v>513</v>
-      </c>
-      <c r="C126" s="23" t="s">
-        <v>11</v>
-      </c>
+        <v>240</v>
+      </c>
+      <c r="B126" s="22" t="s">
+        <v>241</v>
+      </c>
+      <c r="C126" s="27"/>
       <c r="D126" s="24" t="s">
         <v>11</v>
       </c>
       <c r="E126" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="F126" s="70" t="s">
-        <v>499</v>
+      <c r="F126" s="69">
+        <v>3</v>
       </c>
       <c r="G126" s="26"/>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A127" s="21" t="s">
-        <v>240</v>
-      </c>
-      <c r="B127" s="22" t="s">
-        <v>241</v>
+        <v>242</v>
+      </c>
+      <c r="B127" s="65" t="s">
+        <v>514</v>
       </c>
       <c r="C127" s="27"/>
       <c r="D127" s="24" t="s">
@@ -4920,91 +4919,89 @@
       <c r="E127" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="F127" s="69">
+      <c r="F127" s="70" t="s">
+        <v>499</v>
+      </c>
+      <c r="G127" s="26"/>
+    </row>
+    <row r="128" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A128" s="17" t="s">
+        <v>243</v>
+      </c>
+      <c r="B128" s="18" t="s">
+        <v>244</v>
+      </c>
+      <c r="C128" s="19"/>
+      <c r="D128" s="19"/>
+      <c r="E128" s="19"/>
+      <c r="F128" s="75"/>
+      <c r="G128" s="20"/>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A129" s="21" t="s">
+        <v>245</v>
+      </c>
+      <c r="B129" s="22" t="s">
+        <v>246</v>
+      </c>
+      <c r="C129" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D129" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E129" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="F129" s="69">
+        <v>1</v>
+      </c>
+      <c r="G129" s="26"/>
+    </row>
+    <row r="130" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+      <c r="A130" s="21" t="s">
+        <v>247</v>
+      </c>
+      <c r="B130" s="22" t="s">
+        <v>248</v>
+      </c>
+      <c r="C130" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D130" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E130" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="F130" s="69">
         <v>3</v>
       </c>
-      <c r="G127" s="26"/>
-    </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A128" s="21" t="s">
-        <v>242</v>
-      </c>
-      <c r="B128" s="65" t="s">
-        <v>514</v>
-      </c>
-      <c r="C128" s="27"/>
-      <c r="D128" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="E128" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="F128" s="70" t="s">
-        <v>499</v>
-      </c>
-      <c r="G128" s="26"/>
-    </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A129" s="17" t="s">
-        <v>243</v>
-      </c>
-      <c r="B129" s="18" t="s">
-        <v>244</v>
-      </c>
-      <c r="C129" s="19"/>
-      <c r="D129" s="19"/>
-      <c r="E129" s="19"/>
-      <c r="F129" s="75"/>
-      <c r="G129" s="20"/>
-    </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A130" s="21" t="s">
-        <v>245</v>
-      </c>
-      <c r="B130" s="22" t="s">
-        <v>246</v>
-      </c>
-      <c r="C130" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="D130" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="E130" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="F130" s="69">
+      <c r="G130" s="26"/>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A131" s="21" t="s">
+        <v>249</v>
+      </c>
+      <c r="B131" s="22" t="s">
+        <v>250</v>
+      </c>
+      <c r="C131" s="27"/>
+      <c r="D131" s="27"/>
+      <c r="E131" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="F131" s="69">
         <v>1</v>
-      </c>
-      <c r="G130" s="26"/>
-    </row>
-    <row r="131" spans="1:7" ht="26" x14ac:dyDescent="0.15">
-      <c r="A131" s="21" t="s">
-        <v>247</v>
-      </c>
-      <c r="B131" s="22" t="s">
-        <v>248</v>
-      </c>
-      <c r="C131" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="D131" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="E131" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="F131" s="69">
-        <v>3</v>
       </c>
       <c r="G131" s="26"/>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A132" s="21" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="B132" s="22" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="C132" s="27"/>
       <c r="D132" s="27"/>
@@ -5018,13 +5015,15 @@
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A133" s="21" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="B133" s="22" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="C133" s="27"/>
-      <c r="D133" s="27"/>
+      <c r="D133" s="24" t="s">
+        <v>11</v>
+      </c>
       <c r="E133" s="25" t="s">
         <v>11</v>
       </c>
@@ -5035,15 +5034,13 @@
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A134" s="21" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="B134" s="22" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="C134" s="27"/>
-      <c r="D134" s="24" t="s">
-        <v>11</v>
-      </c>
+      <c r="D134" s="27"/>
       <c r="E134" s="25" t="s">
         <v>11</v>
       </c>
@@ -5052,55 +5049,55 @@
       </c>
       <c r="G134" s="26"/>
     </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="135" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A135" s="21" t="s">
-        <v>255</v>
-      </c>
-      <c r="B135" s="22" t="s">
-        <v>256</v>
+        <v>257</v>
+      </c>
+      <c r="B135" s="65" t="s">
+        <v>515</v>
       </c>
       <c r="C135" s="27"/>
-      <c r="D135" s="27"/>
+      <c r="D135" s="24" t="s">
+        <v>11</v>
+      </c>
       <c r="E135" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="F135" s="69">
-        <v>1</v>
+      <c r="F135" s="70" t="s">
+        <v>499</v>
       </c>
       <c r="G135" s="26"/>
     </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="136" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A136" s="21" t="s">
-        <v>257</v>
-      </c>
-      <c r="B136" s="65" t="s">
-        <v>515</v>
-      </c>
-      <c r="C136" s="27"/>
+        <v>258</v>
+      </c>
+      <c r="B136" s="22" t="s">
+        <v>259</v>
+      </c>
+      <c r="C136" s="23" t="s">
+        <v>11</v>
+      </c>
       <c r="D136" s="24" t="s">
         <v>11</v>
       </c>
       <c r="E136" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="F136" s="70" t="s">
-        <v>499</v>
+      <c r="F136" s="69">
+        <v>3</v>
       </c>
       <c r="G136" s="26"/>
     </row>
     <row r="137" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A137" s="21" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="B137" s="22" t="s">
-        <v>259</v>
-      </c>
-      <c r="C137" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="D137" s="24" t="s">
-        <v>11</v>
-      </c>
+        <v>261</v>
+      </c>
+      <c r="C137" s="27"/>
+      <c r="D137" s="27"/>
       <c r="E137" s="25" t="s">
         <v>11</v>
       </c>
@@ -5109,15 +5106,19 @@
       </c>
       <c r="G137" s="26"/>
     </row>
-    <row r="138" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A138" s="21" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="B138" s="22" t="s">
-        <v>261</v>
-      </c>
-      <c r="C138" s="27"/>
-      <c r="D138" s="27"/>
+        <v>263</v>
+      </c>
+      <c r="C138" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D138" s="24" t="s">
+        <v>11</v>
+      </c>
       <c r="E138" s="25" t="s">
         <v>11</v>
       </c>
@@ -5128,10 +5129,10 @@
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A139" s="21" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="B139" s="22" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="C139" s="23" t="s">
         <v>11</v>
@@ -5147,12 +5148,12 @@
       </c>
       <c r="G139" s="26"/>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="140" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A140" s="21" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="B140" s="22" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="C140" s="23" t="s">
         <v>11</v>
@@ -5168,12 +5169,12 @@
       </c>
       <c r="G140" s="26"/>
     </row>
-    <row r="141" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A141" s="21" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="B141" s="22" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="C141" s="23" t="s">
         <v>11</v>
@@ -5190,45 +5191,45 @@
       <c r="G141" s="26"/>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A142" s="21" t="s">
-        <v>268</v>
-      </c>
-      <c r="B142" s="22" t="s">
-        <v>269</v>
-      </c>
-      <c r="C142" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="D142" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="E142" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="F142" s="69">
-        <v>3</v>
-      </c>
-      <c r="G142" s="26"/>
-    </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A143" s="17" t="s">
+      <c r="A142" s="17" t="s">
         <v>270</v>
       </c>
-      <c r="B143" s="18" t="s">
+      <c r="B142" s="18" t="s">
         <v>271</v>
       </c>
-      <c r="C143" s="19"/>
-      <c r="D143" s="19"/>
-      <c r="E143" s="19"/>
-      <c r="F143" s="75"/>
-      <c r="G143" s="20"/>
-    </row>
-    <row r="144" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+      <c r="C142" s="19"/>
+      <c r="D142" s="19"/>
+      <c r="E142" s="19"/>
+      <c r="F142" s="75"/>
+      <c r="G142" s="20"/>
+    </row>
+    <row r="143" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+      <c r="A143" s="21" t="s">
+        <v>272</v>
+      </c>
+      <c r="B143" s="22" t="s">
+        <v>273</v>
+      </c>
+      <c r="C143" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D143" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E143" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="F143" s="69">
+        <v>1</v>
+      </c>
+      <c r="G143" s="26"/>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A144" s="21" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="B144" s="22" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C144" s="23" t="s">
         <v>11</v>
@@ -5246,14 +5247,12 @@
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A145" s="21" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="B145" s="22" t="s">
-        <v>275</v>
-      </c>
-      <c r="C145" s="23" t="s">
-        <v>11</v>
-      </c>
+        <v>277</v>
+      </c>
+      <c r="C145" s="27"/>
       <c r="D145" s="24" t="s">
         <v>11</v>
       </c>
@@ -5261,16 +5260,16 @@
         <v>11</v>
       </c>
       <c r="F145" s="69">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G145" s="26"/>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A146" s="21" t="s">
-        <v>276</v>
-      </c>
-      <c r="B146" s="22" t="s">
-        <v>277</v>
+        <v>278</v>
+      </c>
+      <c r="B146" s="65" t="s">
+        <v>516</v>
       </c>
       <c r="C146" s="27"/>
       <c r="D146" s="24" t="s">
@@ -5279,78 +5278,80 @@
       <c r="E146" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="F146" s="69">
-        <v>2</v>
+      <c r="F146" s="70" t="s">
+        <v>499</v>
       </c>
       <c r="G146" s="26"/>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A147" s="21" t="s">
-        <v>278</v>
-      </c>
-      <c r="B147" s="65" t="s">
-        <v>516</v>
-      </c>
-      <c r="C147" s="27"/>
+        <v>279</v>
+      </c>
+      <c r="B147" s="22" t="s">
+        <v>280</v>
+      </c>
+      <c r="C147" s="23" t="s">
+        <v>11</v>
+      </c>
       <c r="D147" s="24" t="s">
         <v>11</v>
       </c>
       <c r="E147" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="F147" s="70" t="s">
+      <c r="F147" s="69">
+        <v>2</v>
+      </c>
+      <c r="G147" s="26"/>
+    </row>
+    <row r="148" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+      <c r="A148" s="21" t="s">
+        <v>281</v>
+      </c>
+      <c r="B148" s="22" t="s">
+        <v>282</v>
+      </c>
+      <c r="C148" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D148" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E148" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="F148" s="69">
+        <v>3</v>
+      </c>
+      <c r="G148" s="26"/>
+    </row>
+    <row r="149" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A149" s="21" t="s">
+        <v>283</v>
+      </c>
+      <c r="B149" s="65" t="s">
+        <v>517</v>
+      </c>
+      <c r="C149" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D149" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E149" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="F149" s="70" t="s">
         <v>499</v>
-      </c>
-      <c r="G147" s="26"/>
-    </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A148" s="21" t="s">
-        <v>279</v>
-      </c>
-      <c r="B148" s="22" t="s">
-        <v>280</v>
-      </c>
-      <c r="C148" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="D148" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="E148" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="F148" s="69">
-        <v>2</v>
-      </c>
-      <c r="G148" s="26"/>
-    </row>
-    <row r="149" spans="1:7" ht="26" x14ac:dyDescent="0.15">
-      <c r="A149" s="21" t="s">
-        <v>281</v>
-      </c>
-      <c r="B149" s="22" t="s">
-        <v>282</v>
-      </c>
-      <c r="C149" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="D149" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="E149" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="F149" s="69">
-        <v>3</v>
       </c>
       <c r="G149" s="26"/>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A150" s="21" t="s">
-        <v>283</v>
-      </c>
-      <c r="B150" s="65" t="s">
-        <v>517</v>
+        <v>284</v>
+      </c>
+      <c r="B150" s="22" t="s">
+        <v>285</v>
       </c>
       <c r="C150" s="23" t="s">
         <v>11</v>
@@ -5361,124 +5362,122 @@
       <c r="E150" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="F150" s="70" t="s">
-        <v>499</v>
+      <c r="F150" s="69">
+        <v>3</v>
       </c>
       <c r="G150" s="26"/>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A151" s="21" t="s">
-        <v>284</v>
-      </c>
-      <c r="B151" s="22" t="s">
-        <v>285</v>
-      </c>
-      <c r="C151" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="D151" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="E151" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="F151" s="69">
-        <v>3</v>
-      </c>
-      <c r="G151" s="26"/>
+      <c r="A151" s="34" t="s">
+        <v>286</v>
+      </c>
+      <c r="B151" s="35" t="s">
+        <v>287</v>
+      </c>
+      <c r="C151" s="36"/>
+      <c r="D151" s="36"/>
+      <c r="E151" s="36"/>
+      <c r="F151" s="77"/>
+      <c r="G151" s="37"/>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A152" s="34" t="s">
-        <v>286</v>
-      </c>
-      <c r="B152" s="35" t="s">
-        <v>287</v>
-      </c>
-      <c r="C152" s="36"/>
-      <c r="D152" s="36"/>
-      <c r="E152" s="36"/>
-      <c r="F152" s="77"/>
-      <c r="G152" s="37"/>
+      <c r="A152" s="17" t="s">
+        <v>288</v>
+      </c>
+      <c r="B152" s="18" t="s">
+        <v>289</v>
+      </c>
+      <c r="C152" s="19"/>
+      <c r="D152" s="19"/>
+      <c r="E152" s="19"/>
+      <c r="F152" s="75"/>
+      <c r="G152" s="20"/>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A153" s="17" t="s">
-        <v>288</v>
-      </c>
-      <c r="B153" s="18" t="s">
-        <v>289</v>
-      </c>
-      <c r="C153" s="19"/>
-      <c r="D153" s="19"/>
-      <c r="E153" s="19"/>
-      <c r="F153" s="75"/>
-      <c r="G153" s="20"/>
-    </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A153" s="21" t="s">
+        <v>290</v>
+      </c>
+      <c r="B153" s="22" t="s">
+        <v>291</v>
+      </c>
+      <c r="C153" s="27"/>
+      <c r="D153" s="27"/>
+      <c r="E153" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="F153" s="69">
+        <v>2</v>
+      </c>
+      <c r="G153" s="26"/>
+    </row>
+    <row r="154" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A154" s="21" t="s">
-        <v>290</v>
-      </c>
-      <c r="B154" s="22" t="s">
-        <v>291</v>
+        <v>292</v>
+      </c>
+      <c r="B154" s="65" t="s">
+        <v>518</v>
       </c>
       <c r="C154" s="27"/>
       <c r="D154" s="27"/>
       <c r="E154" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="F154" s="69">
+      <c r="F154" s="70" t="s">
+        <v>499</v>
+      </c>
+      <c r="G154" s="26"/>
+    </row>
+    <row r="155" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A155" s="38" t="s">
+        <v>293</v>
+      </c>
+      <c r="B155" s="39" t="s">
+        <v>294</v>
+      </c>
+      <c r="C155" s="40"/>
+      <c r="D155" s="40"/>
+      <c r="E155" s="40"/>
+      <c r="F155" s="75"/>
+      <c r="G155" s="41"/>
+    </row>
+    <row r="156" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A156" s="17" t="s">
+        <v>295</v>
+      </c>
+      <c r="B156" s="18" t="s">
+        <v>296</v>
+      </c>
+      <c r="C156" s="19"/>
+      <c r="D156" s="19"/>
+      <c r="E156" s="19"/>
+      <c r="F156" s="75"/>
+      <c r="G156" s="20"/>
+    </row>
+    <row r="157" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+      <c r="A157" s="21" t="s">
+        <v>297</v>
+      </c>
+      <c r="B157" s="22" t="s">
+        <v>298</v>
+      </c>
+      <c r="C157" s="27"/>
+      <c r="D157" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E157" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="F157" s="69">
         <v>2</v>
       </c>
-      <c r="G154" s="26"/>
-    </row>
-    <row r="155" spans="1:7" ht="26" x14ac:dyDescent="0.15">
-      <c r="A155" s="21" t="s">
-        <v>292</v>
-      </c>
-      <c r="B155" s="65" t="s">
-        <v>518</v>
-      </c>
-      <c r="C155" s="27"/>
-      <c r="D155" s="27"/>
-      <c r="E155" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="F155" s="70" t="s">
-        <v>499</v>
-      </c>
-      <c r="G155" s="26"/>
-    </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A156" s="38" t="s">
-        <v>293</v>
-      </c>
-      <c r="B156" s="39" t="s">
-        <v>294</v>
-      </c>
-      <c r="C156" s="40"/>
-      <c r="D156" s="40"/>
-      <c r="E156" s="40"/>
-      <c r="F156" s="75"/>
-      <c r="G156" s="41"/>
-    </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A157" s="17" t="s">
-        <v>295</v>
-      </c>
-      <c r="B157" s="18" t="s">
-        <v>296</v>
-      </c>
-      <c r="C157" s="19"/>
-      <c r="D157" s="19"/>
-      <c r="E157" s="19"/>
-      <c r="F157" s="75"/>
-      <c r="G157" s="20"/>
+      <c r="G157" s="26"/>
     </row>
     <row r="158" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A158" s="21" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="B158" s="22" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="C158" s="27"/>
       <c r="D158" s="24" t="s">
@@ -5492,44 +5491,46 @@
       </c>
       <c r="G158" s="26"/>
     </row>
-    <row r="159" spans="1:7" ht="26" x14ac:dyDescent="0.15">
-      <c r="A159" s="21" t="s">
-        <v>299</v>
-      </c>
-      <c r="B159" s="22" t="s">
-        <v>300</v>
-      </c>
-      <c r="C159" s="27"/>
-      <c r="D159" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="E159" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="F159" s="69">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A159" s="17" t="s">
+        <v>301</v>
+      </c>
+      <c r="B159" s="18" t="s">
+        <v>302</v>
+      </c>
+      <c r="C159" s="19"/>
+      <c r="D159" s="19"/>
+      <c r="E159" s="19"/>
+      <c r="F159" s="75"/>
+      <c r="G159" s="20"/>
+    </row>
+    <row r="160" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A160" s="21" t="s">
+        <v>303</v>
+      </c>
+      <c r="B160" s="22" t="s">
+        <v>304</v>
+      </c>
+      <c r="C160" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D160" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E160" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="F160" s="69">
         <v>2</v>
       </c>
-      <c r="G159" s="26"/>
-    </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A160" s="17" t="s">
-        <v>301</v>
-      </c>
-      <c r="B160" s="18" t="s">
-        <v>302</v>
-      </c>
-      <c r="C160" s="19"/>
-      <c r="D160" s="19"/>
-      <c r="E160" s="19"/>
-      <c r="F160" s="75"/>
-      <c r="G160" s="20"/>
-    </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="G160" s="26"/>
+    </row>
+    <row r="161" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A161" s="21" t="s">
-        <v>303</v>
-      </c>
-      <c r="B161" s="22" t="s">
-        <v>304</v>
+        <v>305</v>
+      </c>
+      <c r="B161" s="42" t="s">
+        <v>306</v>
       </c>
       <c r="C161" s="23" t="s">
         <v>11</v>
@@ -5547,10 +5548,10 @@
     </row>
     <row r="162" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A162" s="21" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="B162" s="42" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="C162" s="23" t="s">
         <v>11</v>
@@ -5566,12 +5567,12 @@
       </c>
       <c r="G162" s="26"/>
     </row>
-    <row r="163" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A163" s="21" t="s">
-        <v>307</v>
-      </c>
-      <c r="B163" s="42" t="s">
-        <v>308</v>
+        <v>309</v>
+      </c>
+      <c r="B163" s="22" t="s">
+        <v>310</v>
       </c>
       <c r="C163" s="23" t="s">
         <v>11</v>
@@ -5589,10 +5590,10 @@
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A164" s="21" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="B164" s="22" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="C164" s="23" t="s">
         <v>11</v>
@@ -5610,14 +5611,12 @@
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A165" s="21" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="B165" s="22" t="s">
-        <v>312</v>
-      </c>
-      <c r="C165" s="23" t="s">
-        <v>11</v>
-      </c>
+        <v>314</v>
+      </c>
+      <c r="C165" s="27"/>
       <c r="D165" s="24" t="s">
         <v>11</v>
       </c>
@@ -5625,16 +5624,16 @@
         <v>11</v>
       </c>
       <c r="F165" s="69">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G165" s="26"/>
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A166" s="21" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="B166" s="22" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="C166" s="27"/>
       <c r="D166" s="24" t="s">
@@ -5644,18 +5643,20 @@
         <v>11</v>
       </c>
       <c r="F166" s="69">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G166" s="26"/>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A167" s="21" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="B167" s="22" t="s">
-        <v>316</v>
-      </c>
-      <c r="C167" s="27"/>
+        <v>318</v>
+      </c>
+      <c r="C167" s="23" t="s">
+        <v>11</v>
+      </c>
       <c r="D167" s="24" t="s">
         <v>11</v>
       </c>
@@ -5663,16 +5664,16 @@
         <v>11</v>
       </c>
       <c r="F167" s="69">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G167" s="26"/>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A168" s="21" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="B168" s="22" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="C168" s="23" t="s">
         <v>11</v>
@@ -5684,50 +5685,50 @@
         <v>11</v>
       </c>
       <c r="F168" s="69">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G168" s="26"/>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A169" s="21" t="s">
-        <v>319</v>
-      </c>
-      <c r="B169" s="22" t="s">
-        <v>320</v>
-      </c>
-      <c r="C169" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="D169" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="E169" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="F169" s="69">
+      <c r="A169" s="17" t="s">
+        <v>321</v>
+      </c>
+      <c r="B169" s="18" t="s">
+        <v>322</v>
+      </c>
+      <c r="C169" s="19"/>
+      <c r="D169" s="19"/>
+      <c r="E169" s="19"/>
+      <c r="F169" s="75"/>
+      <c r="G169" s="20"/>
+    </row>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A170" s="21" t="s">
+        <v>323</v>
+      </c>
+      <c r="B170" s="22" t="s">
+        <v>324</v>
+      </c>
+      <c r="C170" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D170" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E170" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="F170" s="69">
         <v>2</v>
       </c>
-      <c r="G169" s="26"/>
-    </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A170" s="17" t="s">
-        <v>321</v>
-      </c>
-      <c r="B170" s="18" t="s">
-        <v>322</v>
-      </c>
-      <c r="C170" s="19"/>
-      <c r="D170" s="19"/>
-      <c r="E170" s="19"/>
-      <c r="F170" s="75"/>
-      <c r="G170" s="20"/>
+      <c r="G170" s="26"/>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A171" s="21" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="B171" s="22" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="C171" s="23" t="s">
         <v>11</v>
@@ -5745,10 +5746,10 @@
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A172" s="21" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="B172" s="22" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="C172" s="23" t="s">
         <v>11</v>
@@ -5766,10 +5767,10 @@
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A173" s="21" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="B173" s="22" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="C173" s="23" t="s">
         <v>11</v>
@@ -5785,16 +5786,14 @@
       </c>
       <c r="G173" s="26"/>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="174" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A174" s="21" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="B174" s="22" t="s">
-        <v>330</v>
-      </c>
-      <c r="C174" s="23" t="s">
-        <v>11</v>
-      </c>
+        <v>332</v>
+      </c>
+      <c r="C174" s="27"/>
       <c r="D174" s="24" t="s">
         <v>11</v>
       </c>
@@ -5806,12 +5805,12 @@
       </c>
       <c r="G174" s="26"/>
     </row>
-    <row r="175" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A175" s="21" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="B175" s="22" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="C175" s="27"/>
       <c r="D175" s="24" t="s">
@@ -5827,12 +5826,14 @@
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A176" s="21" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="B176" s="22" t="s">
-        <v>334</v>
-      </c>
-      <c r="C176" s="27"/>
+        <v>336</v>
+      </c>
+      <c r="C176" s="23" t="s">
+        <v>11</v>
+      </c>
       <c r="D176" s="24" t="s">
         <v>11</v>
       </c>
@@ -5844,19 +5845,15 @@
       </c>
       <c r="G176" s="26"/>
     </row>
-    <row r="177" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="177" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A177" s="21" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="B177" s="22" t="s">
-        <v>336</v>
-      </c>
-      <c r="C177" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="D177" s="24" t="s">
-        <v>11</v>
-      </c>
+        <v>338</v>
+      </c>
+      <c r="C177" s="27"/>
+      <c r="D177" s="27"/>
       <c r="E177" s="25" t="s">
         <v>11</v>
       </c>
@@ -5865,15 +5862,19 @@
       </c>
       <c r="G177" s="26"/>
     </row>
-    <row r="178" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="178" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A178" s="21" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="B178" s="22" t="s">
-        <v>338</v>
-      </c>
-      <c r="C178" s="27"/>
-      <c r="D178" s="27"/>
+        <v>340</v>
+      </c>
+      <c r="C178" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D178" s="24" t="s">
+        <v>11</v>
+      </c>
       <c r="E178" s="25" t="s">
         <v>11</v>
       </c>
@@ -5884,33 +5885,33 @@
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A179" s="21" t="s">
-        <v>339</v>
-      </c>
-      <c r="B179" s="22" t="s">
-        <v>340</v>
-      </c>
-      <c r="C179" s="23" t="s">
-        <v>11</v>
-      </c>
+        <v>341</v>
+      </c>
+      <c r="B179" s="65" t="s">
+        <v>514</v>
+      </c>
+      <c r="C179" s="27"/>
       <c r="D179" s="24" t="s">
         <v>11</v>
       </c>
       <c r="E179" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="F179" s="69">
-        <v>2</v>
+      <c r="F179" s="70" t="s">
+        <v>499</v>
       </c>
       <c r="G179" s="26"/>
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A180" s="21" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="B180" s="65" t="s">
-        <v>514</v>
-      </c>
-      <c r="C180" s="27"/>
+        <v>519</v>
+      </c>
+      <c r="C180" s="23" t="s">
+        <v>11</v>
+      </c>
       <c r="D180" s="24" t="s">
         <v>11</v>
       </c>
@@ -5923,45 +5924,45 @@
       <c r="G180" s="26"/>
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A181" s="21" t="s">
-        <v>342</v>
-      </c>
-      <c r="B181" s="65" t="s">
-        <v>519</v>
-      </c>
-      <c r="C181" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="D181" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="E181" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="F181" s="70" t="s">
-        <v>499</v>
-      </c>
-      <c r="G181" s="26"/>
+      <c r="A181" s="17" t="s">
+        <v>343</v>
+      </c>
+      <c r="B181" s="18" t="s">
+        <v>344</v>
+      </c>
+      <c r="C181" s="19"/>
+      <c r="D181" s="19"/>
+      <c r="E181" s="19"/>
+      <c r="F181" s="75"/>
+      <c r="G181" s="20"/>
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A182" s="17" t="s">
-        <v>343</v>
-      </c>
-      <c r="B182" s="18" t="s">
-        <v>344</v>
-      </c>
-      <c r="C182" s="19"/>
-      <c r="D182" s="19"/>
-      <c r="E182" s="19"/>
-      <c r="F182" s="75"/>
-      <c r="G182" s="20"/>
+      <c r="A182" s="21" t="s">
+        <v>345</v>
+      </c>
+      <c r="B182" s="22" t="s">
+        <v>346</v>
+      </c>
+      <c r="C182" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D182" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E182" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="F182" s="69">
+        <v>3</v>
+      </c>
+      <c r="G182" s="26"/>
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A183" s="21" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="B183" s="22" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="C183" s="23" t="s">
         <v>11</v>
@@ -5979,10 +5980,10 @@
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A184" s="21" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="B184" s="22" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="C184" s="23" t="s">
         <v>11</v>
@@ -6000,10 +6001,10 @@
     </row>
     <row r="185" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A185" s="21" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B185" s="22" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="C185" s="23" t="s">
         <v>11</v>
@@ -6019,12 +6020,12 @@
       </c>
       <c r="G185" s="26"/>
     </row>
-    <row r="186" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="186" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A186" s="21" t="s">
-        <v>351</v>
-      </c>
-      <c r="B186" s="22" t="s">
-        <v>352</v>
+        <v>353</v>
+      </c>
+      <c r="B186" s="65" t="s">
+        <v>520</v>
       </c>
       <c r="C186" s="23" t="s">
         <v>11</v>
@@ -6035,38 +6036,38 @@
       <c r="E186" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="F186" s="69">
+      <c r="F186" s="70" t="s">
+        <v>499</v>
+      </c>
+      <c r="G186" s="26"/>
+    </row>
+    <row r="187" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+      <c r="A187" s="21" t="s">
+        <v>354</v>
+      </c>
+      <c r="B187" s="22" t="s">
+        <v>355</v>
+      </c>
+      <c r="C187" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D187" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E187" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="F187" s="69">
         <v>3</v>
-      </c>
-      <c r="G186" s="26"/>
-    </row>
-    <row r="187" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A187" s="21" t="s">
-        <v>353</v>
-      </c>
-      <c r="B187" s="65" t="s">
-        <v>520</v>
-      </c>
-      <c r="C187" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="D187" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="E187" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="F187" s="70" t="s">
-        <v>499</v>
       </c>
       <c r="G187" s="26"/>
     </row>
     <row r="188" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A188" s="21" t="s">
-        <v>354</v>
-      </c>
-      <c r="B188" s="22" t="s">
-        <v>355</v>
+        <v>356</v>
+      </c>
+      <c r="B188" s="65" t="s">
+        <v>521</v>
       </c>
       <c r="C188" s="23" t="s">
         <v>11</v>
@@ -6077,38 +6078,36 @@
       <c r="E188" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="F188" s="69">
+      <c r="F188" s="70" t="s">
+        <v>499</v>
+      </c>
+      <c r="G188" s="26"/>
+    </row>
+    <row r="189" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A189" s="21" t="s">
+        <v>357</v>
+      </c>
+      <c r="B189" s="22" t="s">
+        <v>358</v>
+      </c>
+      <c r="C189" s="27"/>
+      <c r="D189" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E189" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="F189" s="69">
         <v>3</v>
       </c>
-      <c r="G188" s="26"/>
-    </row>
-    <row r="189" spans="1:7" ht="26" x14ac:dyDescent="0.15">
-      <c r="A189" s="21" t="s">
-        <v>356</v>
-      </c>
-      <c r="B189" s="65" t="s">
-        <v>521</v>
-      </c>
-      <c r="C189" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="D189" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="E189" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="F189" s="70" t="s">
-        <v>499</v>
-      </c>
       <c r="G189" s="26"/>
     </row>
-    <row r="190" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="190" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A190" s="21" t="s">
-        <v>357</v>
-      </c>
-      <c r="B190" s="22" t="s">
-        <v>358</v>
+        <v>359</v>
+      </c>
+      <c r="B190" s="65" t="s">
+        <v>522</v>
       </c>
       <c r="C190" s="27"/>
       <c r="D190" s="24" t="s">
@@ -6117,17 +6116,17 @@
       <c r="E190" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="F190" s="69">
-        <v>3</v>
+      <c r="F190" s="70" t="s">
+        <v>499</v>
       </c>
       <c r="G190" s="26"/>
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A191" s="21" t="s">
-        <v>359</v>
-      </c>
-      <c r="B191" s="65" t="s">
-        <v>522</v>
+        <v>360</v>
+      </c>
+      <c r="B191" s="22" t="s">
+        <v>361</v>
       </c>
       <c r="C191" s="27"/>
       <c r="D191" s="24" t="s">
@@ -6136,53 +6135,53 @@
       <c r="E191" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="F191" s="70" t="s">
-        <v>499</v>
+      <c r="F191" s="69">
+        <v>3</v>
       </c>
       <c r="G191" s="26"/>
     </row>
     <row r="192" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A192" s="21" t="s">
-        <v>360</v>
-      </c>
-      <c r="B192" s="22" t="s">
-        <v>361</v>
-      </c>
-      <c r="C192" s="27"/>
-      <c r="D192" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="E192" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="F192" s="69">
+      <c r="A192" s="17" t="s">
+        <v>362</v>
+      </c>
+      <c r="B192" s="18" t="s">
+        <v>363</v>
+      </c>
+      <c r="C192" s="19"/>
+      <c r="D192" s="19"/>
+      <c r="E192" s="19"/>
+      <c r="F192" s="75"/>
+      <c r="G192" s="20"/>
+    </row>
+    <row r="193" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+      <c r="A193" s="21" t="s">
+        <v>364</v>
+      </c>
+      <c r="B193" s="22" t="s">
+        <v>365</v>
+      </c>
+      <c r="C193" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="D193" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E193" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="F193" s="69">
         <v>3</v>
       </c>
-      <c r="G192" s="26"/>
-    </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A193" s="17" t="s">
-        <v>362</v>
-      </c>
-      <c r="B193" s="18" t="s">
-        <v>363</v>
-      </c>
-      <c r="C193" s="19"/>
-      <c r="D193" s="19"/>
-      <c r="E193" s="19"/>
-      <c r="F193" s="75"/>
-      <c r="G193" s="20"/>
+      <c r="G193" s="26"/>
     </row>
     <row r="194" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A194" s="21" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="B194" s="22" t="s">
-        <v>365</v>
-      </c>
-      <c r="C194" s="23" t="s">
-        <v>11</v>
-      </c>
+        <v>367</v>
+      </c>
+      <c r="C194" s="27"/>
       <c r="D194" s="24" t="s">
         <v>11</v>
       </c>
@@ -6196,10 +6195,10 @@
     </row>
     <row r="195" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A195" s="21" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="B195" s="22" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="C195" s="27"/>
       <c r="D195" s="24" t="s">
@@ -6213,12 +6212,12 @@
       </c>
       <c r="G195" s="26"/>
     </row>
-    <row r="196" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="196" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A196" s="21" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="B196" s="22" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="C196" s="27"/>
       <c r="D196" s="24" t="s">
@@ -6234,10 +6233,10 @@
     </row>
     <row r="197" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A197" s="21" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="B197" s="22" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="C197" s="27"/>
       <c r="D197" s="24" t="s">
@@ -6251,17 +6250,15 @@
       </c>
       <c r="G197" s="26"/>
     </row>
-    <row r="198" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="198" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A198" s="21" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="B198" s="22" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="C198" s="27"/>
-      <c r="D198" s="24" t="s">
-        <v>11</v>
-      </c>
+      <c r="D198" s="27"/>
       <c r="E198" s="25" t="s">
         <v>11</v>
       </c>
@@ -6272,10 +6269,10 @@
     </row>
     <row r="199" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A199" s="21" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="B199" s="22" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="C199" s="27"/>
       <c r="D199" s="27"/>
@@ -6289,10 +6286,10 @@
     </row>
     <row r="200" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A200" s="21" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="B200" s="22" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="C200" s="27"/>
       <c r="D200" s="27"/>
@@ -6306,10 +6303,10 @@
     </row>
     <row r="201" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A201" s="21" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="B201" s="22" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="C201" s="27"/>
       <c r="D201" s="27"/>
@@ -6321,38 +6318,30 @@
       </c>
       <c r="G201" s="26"/>
     </row>
-    <row r="202" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A202" s="21" t="s">
-        <v>380</v>
-      </c>
-      <c r="B202" s="22" t="s">
-        <v>381</v>
+    <row r="202" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+      <c r="A202" s="46" t="s">
+        <v>523</v>
+      </c>
+      <c r="B202" s="65" t="s">
+        <v>524</v>
       </c>
       <c r="C202" s="27"/>
       <c r="D202" s="27"/>
       <c r="E202" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="F202" s="69">
-        <v>3</v>
-      </c>
-      <c r="G202" s="26"/>
-    </row>
-    <row r="203" spans="1:7" ht="26" x14ac:dyDescent="0.15">
-      <c r="A203" s="46" t="s">
-        <v>523</v>
-      </c>
-      <c r="B203" s="65" t="s">
-        <v>524</v>
-      </c>
-      <c r="C203" s="27"/>
-      <c r="D203" s="27"/>
-      <c r="E203" s="25" t="s">
-        <v>11</v>
-      </c>
-      <c r="F203" s="70" t="s">
+      <c r="F202" s="70" t="s">
         <v>499</v>
       </c>
+      <c r="G202" s="44"/>
+    </row>
+    <row r="203" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A203" s="43"/>
+      <c r="B203" s="15"/>
+      <c r="C203" s="15"/>
+      <c r="D203" s="15"/>
+      <c r="E203" s="15"/>
+      <c r="F203" s="78"/>
       <c r="G203" s="44"/>
     </row>
     <row r="204" spans="1:7" x14ac:dyDescent="0.15">
@@ -13402,18 +13391,9 @@
       <c r="F986" s="78"/>
       <c r="G986" s="44"/>
     </row>
-    <row r="987" spans="1:7" x14ac:dyDescent="0.15">
-      <c r="A987" s="43"/>
-      <c r="B987" s="15"/>
-      <c r="C987" s="15"/>
-      <c r="D987" s="15"/>
-      <c r="E987" s="15"/>
-      <c r="F987" s="78"/>
-      <c r="G987" s="44"/>
-    </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G203">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G202" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>$R$2:$R$4</formula1>
     </dataValidation>
   </dataValidations>
@@ -13423,7 +13403,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -13692,7 +13672,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="26" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:5" ht="39" x14ac:dyDescent="0.15">
       <c r="A16" s="46">
         <v>4.13</v>
       </c>
@@ -13845,7 +13825,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="26" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:5" ht="39" x14ac:dyDescent="0.15">
       <c r="A25" s="46">
         <v>5.19</v>
       </c>
@@ -14047,7 +14027,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:5" ht="26" x14ac:dyDescent="0.15">
       <c r="A37" s="46">
         <v>10.199999999999999</v>
       </c>
@@ -14075,7 +14055,7 @@
       <c r="D38" s="27"/>
       <c r="E38" s="27"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:5" ht="26" x14ac:dyDescent="0.15">
       <c r="A39" s="46">
         <v>10.9</v>
       </c>
@@ -20987,10 +20967,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:A31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>

</xml_diff>